<commit_message>
* Spell Mistake issues fixed * Created bi-direction relation. * Created API to list campaign, campaing info and campaign Info with lead * Created the Viewmodel to avoid unnecessary traffic * Created the Campaign List page - Angular * Support to create campaign with simple filter - Angular * Added necessary models and View Models - Angular * Upload Lead excel file update to support Pincode and Locality.
</commit_message>
<xml_diff>
--- a/src/addon365.Web.API/Resources/LeadTemplate.xlsx
+++ b/src/addon365.Web.API/Resources/LeadTemplate.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Me\Addon\BikeShowRoom\b1ke-sh0wr00m\src\addon365.Web.API\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8606F48A-C235-421C-A078-CCD0776405DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DB345D2B-0574-42AB-9040-1A5D540BCBF4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8105" tabRatio="551" xr2:uid="{4AD98230-DE9E-43EB-897A-5902C318DD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="LeadSource" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>BusinessName</t>
   </si>
@@ -74,6 +74,45 @@
   </si>
   <si>
     <t>Proprietor Name</t>
+  </si>
+  <si>
+    <t>Districts</t>
+  </si>
+  <si>
+    <t>Cuddalore</t>
+  </si>
+  <si>
+    <t>Vellore</t>
+  </si>
+  <si>
+    <t>Tiruvamur</t>
+  </si>
+  <si>
+    <t>Kattiyampalayam</t>
+  </si>
+  <si>
+    <t>Tamilnadu</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>Pincodes</t>
+  </si>
+  <si>
+    <t>Localities</t>
+  </si>
+  <si>
+    <t>SubDistricts</t>
+  </si>
+  <si>
+    <t>Panruti</t>
+  </si>
+  <si>
+    <t>Virudhachalam</t>
   </si>
 </sst>
 </file>
@@ -183,6 +222,56 @@
   <autoFilter ref="A1:A4" xr:uid="{159EB3B4-92AF-4536-821E-DFE3839CD609}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{11D44F56-6B85-4BCF-BB8E-B3E24F85D32A}" name="LeadSource"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{01AEB12E-B451-44CF-9DAA-5C0ED8EDD69F}" name="Table3" displayName="Table3" ref="D1:D3" totalsRowShown="0">
+  <autoFilter ref="D1:D3" xr:uid="{C1CDB901-8681-4308-B768-5AF1D8D559C8}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{60DF628F-C7D3-4A83-84E0-83BF86AA1F25}" name="Districts"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3F6438EC-717A-4EB2-950D-11937BEE18A2}" name="Table4" displayName="Table4" ref="F1:F3" totalsRowShown="0">
+  <autoFilter ref="F1:F3" xr:uid="{4B025A58-53B3-40D8-8E7C-AF3831886C1E}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CB0C4E6C-3F2D-4096-B019-0E5AE30D6E1C}" name="Localities"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{26AF2F46-C4E6-456F-B1B9-80A7A4694601}" name="Table5" displayName="Table5" ref="H1:H3" totalsRowShown="0">
+  <autoFilter ref="H1:H3" xr:uid="{86B1599E-2DAD-4B0A-9B9F-DBC159492A61}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{040F5A8D-C2BA-4651-B813-E7C552A6179F}" name="Pincodes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F9BC35AC-E9B6-4105-B8EB-B1F0E33C9024}" name="Table6" displayName="Table6" ref="J1:J3" totalsRowShown="0">
+  <autoFilter ref="J1:J3" xr:uid="{13C9BB4C-45E7-4C3B-913C-8C1ECEA0D2B8}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B81FDBEC-296E-407A-8F90-12C764715367}" name="States"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9EBA0DE9-71B0-41F1-918E-ECA523EFF28B}" name="Table7" displayName="Table7" ref="L1:L3" totalsRowShown="0">
+  <autoFilter ref="L1:L3" xr:uid="{3C696553-2E44-441B-8422-69F568625F61}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CFA924D2-CF6B-461F-B77A-A1D9842586AB}" name="SubDistricts"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -487,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DD7041-55E8-45E8-8B8E-231405707AAF}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -554,12 +643,30 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92222375-5144-4088-BB3C-B2A32C0565D6}">
           <x14:formula1>
-            <xm:f>LeadSource!$A$2:$A$4</xm:f>
+            <xm:f>Data!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>M2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{CAE8584C-D4D8-4ECE-8CD6-1624F34FD30A}">
+          <x14:formula1>
+            <xm:f>Data!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACEEDDF4-DE9D-4726-AF79-573DCFF55BBE}">
+          <x14:formula1>
+            <xm:f>Data!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3B8A8950-2835-4C73-850B-D55CF0FCEFAC}">
+          <x14:formula1>
+            <xm:f>Data!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -569,41 +676,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865A648E-2F5D-4905-A3EF-92B470E94E43}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9.76953125" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>11</v>
       </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>607106</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>607108</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>